<commit_message>
Datos en excel Listo
</commit_message>
<xml_diff>
--- a/HORARIOS.xlsx
+++ b/HORARIOS.xlsx
@@ -11,14 +11,16 @@
     <sheet name="M1 - 301" sheetId="2" r:id="rId2"/>
     <sheet name="M1 - 302" sheetId="3" r:id="rId3"/>
     <sheet name="M1 - 303" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
+    <sheet name="M1 - 304" sheetId="5" r:id="rId5"/>
+    <sheet name="M1 - 305" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="17">
   <si>
     <t>Lunes</t>
   </si>
@@ -59,25 +61,16 @@
     <t>Bloque 7</t>
   </si>
   <si>
-    <t xml:space="preserve">Celda </t>
-  </si>
-  <si>
-    <t xml:space="preserve">elda </t>
-  </si>
-  <si>
-    <t xml:space="preserve">lda </t>
-  </si>
-  <si>
-    <t xml:space="preserve">da </t>
-  </si>
-  <si>
-    <t xml:space="preserve">a </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t/>
+    <t>2998-MATC8031</t>
+  </si>
+  <si>
+    <t>2995-INFB8010</t>
+  </si>
+  <si>
+    <t>2993-INF64000</t>
+  </si>
+  <si>
+    <t>2994-INF79800</t>
   </si>
 </sst>
 </file>
@@ -418,37 +411,151 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="2:8">
       <c r="B4" t="s">
         <v>7</v>
       </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" spans="2:8">
       <c r="B5" t="s">
         <v>8</v>
       </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" spans="2:8">
       <c r="B6" t="s">
         <v>9</v>
       </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" spans="2:8">
       <c r="B7" t="s">
         <v>10</v>
       </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="2:8">
       <c r="B8" t="s">
         <v>11</v>
       </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="9" spans="2:8">
       <c r="B9" t="s">
         <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -486,37 +593,151 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="2:8">
       <c r="B4" t="s">
         <v>7</v>
       </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" spans="2:8">
       <c r="B5" t="s">
         <v>8</v>
       </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" spans="2:8">
       <c r="B6" t="s">
         <v>9</v>
       </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" spans="2:8">
       <c r="B7" t="s">
         <v>10</v>
       </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="2:8">
       <c r="B8" t="s">
         <v>11</v>
       </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="9" spans="2:8">
       <c r="B9" t="s">
         <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -553,37 +774,151 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="2:8">
       <c r="B4" t="s">
         <v>7</v>
       </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" spans="2:8">
       <c r="B5" t="s">
         <v>8</v>
       </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" spans="2:8">
       <c r="B6" t="s">
         <v>9</v>
       </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" spans="2:8">
       <c r="B7" t="s">
         <v>10</v>
       </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="2:8">
       <c r="B8" t="s">
         <v>11</v>
       </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="9" spans="2:8">
       <c r="B9" t="s">
         <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -620,37 +955,151 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="2:8">
       <c r="B4" t="s">
         <v>7</v>
       </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" spans="2:8">
       <c r="B5" t="s">
         <v>8</v>
       </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" spans="2:8">
       <c r="B6" t="s">
         <v>9</v>
       </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" spans="2:8">
       <c r="B7" t="s">
         <v>10</v>
       </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="2:8">
       <c r="B8" t="s">
         <v>11</v>
       </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="9" spans="2:8">
       <c r="B9" t="s">
         <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -659,6 +1108,368 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:H9"/>
+  <sheetFormatPr/>
+  <sheetData>
+    <row r="2" spans="3:8">
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8">
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8">
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8">
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8">
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:H9"/>
+  <sheetFormatPr/>
+  <sheetData>
+    <row r="2" spans="3:8">
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8">
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8">
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8">
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8">
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetFormatPr/>
   <sheetData/>

</xml_diff>